<commit_message>
youtube form with accounts done
</commit_message>
<xml_diff>
--- a/Files/email_password.xlsx
+++ b/Files/email_password.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddyg\Desktop\FYP\GitHub\fyp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC6CDF-9F90-41B3-A87F-2AECBFB09D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D786487B-A5ED-4BD4-94E3-F4A01220160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="408" yWindow="264" windowWidth="17280" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>samira_raad2000@outlook.com</t>
   </si>
@@ -52,6 +52,30 @@
   </si>
   <si>
     <t>marcelle.haddad@outlook.com</t>
+  </si>
+  <si>
+    <t>bahsa.leb@gmail.com</t>
+  </si>
+  <si>
+    <t>Samira Raad</t>
+  </si>
+  <si>
+    <t>Samir Hanna</t>
+  </si>
+  <si>
+    <t>Marcelle Hanna</t>
+  </si>
+  <si>
+    <t>Didi Hanna</t>
+  </si>
+  <si>
+    <t>Marcelle Haddad</t>
+  </si>
+  <si>
+    <t>Michael Merri</t>
+  </si>
+  <si>
+    <t>Bahsa Lebron</t>
   </si>
 </sst>
 </file>
@@ -380,74 +404,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{41F1C30C-D00C-4FC4-A4D6-C814D1B64353}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{07905395-DBD7-4E24-AAD7-5C0AB5F1BA8D}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{5A0F5064-7D44-4783-AC31-317BD4427B62}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{F3CF579B-5861-41D4-AA37-AA30156A51AD}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{08F7C063-037E-4679-82BD-E51AB2CC7800}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{94B6553B-320B-4146-AE05-6C615E45D1FF}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{41F1C30C-D00C-4FC4-A4D6-C814D1B64353}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{07905395-DBD7-4E24-AAD7-5C0AB5F1BA8D}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{5A0F5064-7D44-4783-AC31-317BD4427B62}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{F3CF579B-5861-41D4-AA37-AA30156A51AD}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{08F7C063-037E-4679-82BD-E51AB2CC7800}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{94B6553B-320B-4146-AE05-6C615E45D1FF}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{BB7F0289-1DA4-416E-8D41-C78F34CF83E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>